<commit_message>
Delete check in account group (Build 467)
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint25Plan.xlsx
+++ b/doc/Planning/Sprint25Plan.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
   <si>
     <t>هدف کاری</t>
   </si>
@@ -176,6 +176,36 @@
   </si>
   <si>
     <t>انجام فیلترهای مختلف روی لاگ های عملیاتی در برنامه</t>
+  </si>
+  <si>
+    <t>گزارش های سیستم مالی</t>
+  </si>
+  <si>
+    <t>تهیه اطلاعات گزارش دفتر روزنامه (مطابق ردیف های سند) در سرویس</t>
+  </si>
+  <si>
+    <t>مشاهده اطلاعات گزارش دفتر روزنامه در فرم گزارشی جدید در برنامه</t>
+  </si>
+  <si>
+    <t>تهیه اطلاعات گزارش دفتر حساب (مطابق ردیف های سند، برای مولفه حساب) در سرویس</t>
+  </si>
+  <si>
+    <t>مشاهده اطلاعات گزارش دفتر حساب در فرم گزارشی جدید در برنامه</t>
+  </si>
+  <si>
+    <t>طراحی گزارش دفتر روزنامه در محیط طراحی و یکپارچه سازی در برنامه</t>
+  </si>
+  <si>
+    <t>طراحی گزارش دفتر حساب در محیط طراحی و یکپارچه سازی در برنامه</t>
+  </si>
+  <si>
+    <t>رفع اشکالات موجود</t>
+  </si>
+  <si>
+    <t>رفع اشکال گروه بندی حسابها در گزارش سند حسابداری - فرم مرسوم</t>
+  </si>
+  <si>
+    <t>رفع اشکال گروه بندی حسابها در گزارش سند حسابداری - با سطوح شناور</t>
   </si>
 </sst>
 </file>
@@ -1044,8 +1074,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E31" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
-  <autoFilter ref="A2:E31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E32" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+  <autoFilter ref="A2:E32"/>
   <tableColumns count="5">
     <tableColumn id="1" name="هدف کاری" dataDxfId="43"/>
     <tableColumn id="2" name="قابلیت" dataDxfId="42"/>
@@ -1377,10 +1407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1612,8 +1642,12 @@
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="4"/>
+      <c r="A20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="C20" s="5">
         <v>1</v>
       </c>
@@ -1622,7 +1656,9 @@
     </row>
     <row r="21" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="C21" s="5">
         <v>1</v>
       </c>
@@ -1631,16 +1667,20 @@
     </row>
     <row r="22" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
-      <c r="B22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="C22" s="5">
         <v>1</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
-      <c r="B23" s="4"/>
+      <c r="B23" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="C23" s="5">
         <v>1</v>
       </c>
@@ -1649,7 +1689,9 @@
     </row>
     <row r="24" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
-      <c r="B24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="C24" s="5">
         <v>1</v>
       </c>
@@ -1658,7 +1700,9 @@
     </row>
     <row r="25" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
-      <c r="B25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="C25" s="5">
         <v>1</v>
       </c>
@@ -1667,57 +1711,65 @@
     </row>
     <row r="26" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="4"/>
+      <c r="B26" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="C26" s="5">
         <v>1</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="5">
-        <v>1</v>
-      </c>
-      <c r="D27" s="5" t="s">
+      <c r="C28" s="5">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="5">
-        <v>1</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="5">
-        <v>1</v>
-      </c>
-      <c r="D29" s="5" t="s">
+      <c r="C30" s="5">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1727,9 +1779,16 @@
       <c r="D31" s="5"/>
       <c r="E31" s="4"/>
     </row>
+    <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="4"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:C23 C3:C16 C26:C31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:C23 C3:C16 C28:C32">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Disabled UseLeafAccounts option in Settings API (Build 471)
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint25Plan.xlsx
+++ b/doc/Planning/Sprint25Plan.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>هدف کاری</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>رفع اشکال گروه بندی حسابها در گزارش سند حسابداری - با سطوح شناور</t>
+  </si>
+  <si>
+    <t>حذف گزینه ارتباطات بردار حساب برای سرفصل حسابداری</t>
+  </si>
+  <si>
+    <t>با توجه به تصمیم گیری انجام شده در جلسه دموی اسپرینت قبل در مورد عدم پشتیبانی از گزینه "برقراری ارتباطات در آخرین سطح سرفصل حسابداری"</t>
   </si>
 </sst>
 </file>
@@ -1074,8 +1080,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E32" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
-  <autoFilter ref="A2:E32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E33" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+  <autoFilter ref="A2:E33"/>
   <tableColumns count="5">
     <tableColumn id="1" name="هدف کاری" dataDxfId="43"/>
     <tableColumn id="2" name="قابلیت" dataDxfId="42"/>
@@ -1407,10 +1413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,49 +1597,51 @@
       <c r="D15" s="5"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>41</v>
-      </c>
+    <row r="16" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
       <c r="B16" s="4" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="B17" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C18" s="5">
         <v>1</v>
       </c>
       <c r="D18" s="5"/>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
@@ -1642,11 +1650,9 @@
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="A20" s="7"/>
       <c r="B20" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
@@ -1655,9 +1661,11 @@
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="B21" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="5">
         <v>1</v>
@@ -1668,7 +1676,7 @@
     <row r="22" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="4" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C22" s="5">
         <v>1</v>
@@ -1676,10 +1684,10 @@
       <c r="D22" s="5"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="5">
         <v>1</v>
@@ -1687,10 +1695,10 @@
       <c r="D23" s="5"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C24" s="5">
         <v>1</v>
@@ -1701,7 +1709,7 @@
     <row r="25" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C25" s="5">
         <v>1</v>
@@ -1712,7 +1720,7 @@
     <row r="26" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="5">
         <v>1</v>
@@ -1723,7 +1731,7 @@
     <row r="27" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C27" s="5">
         <v>1</v>
@@ -1731,52 +1739,56 @@
       <c r="D27" s="5"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+    <row r="28" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="5">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="5">
-        <v>1</v>
-      </c>
-      <c r="D28" s="5" t="s">
+      <c r="C29" s="5">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="5">
-        <v>1</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="5">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="5">
-        <v>1</v>
-      </c>
-      <c r="D30" s="5" t="s">
+      <c r="C31" s="5">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E30" s="4"/>
-    </row>
-    <row r="31" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
       <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1786,9 +1798,16 @@
       <c r="D32" s="5"/>
       <c r="E32" s="4"/>
     </row>
+    <row r="33" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="4"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:C23 C3:C16 C28:C32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20:C24 C3:C17 C29:C33">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Reading accounts of an account group (Build 482)
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint25Plan.xlsx
+++ b/doc/Planning/Sprint25Plan.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
   <si>
     <t>هدف کاری</t>
   </si>
@@ -212,6 +212,21 @@
   </si>
   <si>
     <t>با توجه به تصمیم گیری انجام شده در جلسه دموی اسپرینت قبل در مورد عدم پشتیبانی از گزینه "برقراری ارتباطات در آخرین سطح سرفصل حسابداری"</t>
+  </si>
+  <si>
+    <t>حذف رکوردهای ارتباطات برای شناورهای زیرمجموعه در سرویس</t>
+  </si>
+  <si>
+    <t>حذف رکوردهای ارتباطات برای مراکز هزینه زیرمجموعه در سرویس</t>
+  </si>
+  <si>
+    <t>حذف رکوردهای ارتباطات برای پروژه های زیرمجموعه در سرویس</t>
+  </si>
+  <si>
+    <t>منظور عملکرد مشابه تدبیر در مواردی است که ارتباطات موجود با سطوح ماقبل آخر قطع می شوند.</t>
+  </si>
+  <si>
+    <t>خواندن حساب های زیرمجموعه یک گروه حساب در سرویس</t>
   </si>
 </sst>
 </file>
@@ -1080,8 +1095,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E33" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
-  <autoFilter ref="A2:E33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E37" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+  <autoFilter ref="A2:E37"/>
   <tableColumns count="5">
     <tableColumn id="1" name="هدف کاری" dataDxfId="43"/>
     <tableColumn id="2" name="قابلیت" dataDxfId="42"/>
@@ -1413,11 +1428,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1510,7 +1523,7 @@
     <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="4" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
@@ -1521,7 +1534,7 @@
     <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -1529,67 +1542,71 @@
       <c r="D9" s="5"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4" t="s">
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="4" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C14" s="5">
         <v>1</v>
       </c>
       <c r="D14" s="5"/>
-      <c r="E14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="4" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="C15" s="5">
         <v>1</v>
@@ -1597,51 +1614,45 @@
       <c r="D15" s="5"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
       </c>
       <c r="D16" s="5"/>
-      <c r="E16" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
       <c r="B17" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C18" s="5">
         <v>1</v>
       </c>
       <c r="D18" s="5"/>
-      <c r="E18" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
@@ -1649,67 +1660,75 @@
       <c r="D19" s="5"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
       </c>
       <c r="D20" s="5"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C21" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="5"/>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="4" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C22" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" s="5"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C23" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C24" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="B25" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C25" s="5">
         <v>1</v>
@@ -1720,7 +1739,7 @@
     <row r="26" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C26" s="5">
         <v>1</v>
@@ -1731,7 +1750,7 @@
     <row r="27" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C27" s="5">
         <v>1</v>
@@ -1739,10 +1758,10 @@
       <c r="D27" s="5"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C28" s="5">
         <v>1</v>
@@ -1750,64 +1769,108 @@
       <c r="D28" s="5"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>55</v>
-      </c>
+    <row r="29" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
       <c r="B29" s="4" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="C29" s="5">
         <v>1</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="D29" s="5"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="4" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="C30" s="5">
         <v>1</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="D30" s="5"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="4" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="C31" s="5">
         <v>1</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="D31" s="5"/>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="5"/>
+      <c r="B32" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1</v>
+      </c>
       <c r="D32" s="5"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+    <row r="33" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="5">
+        <v>1</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="5">
+        <v>1</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20:C24 C3:C17 C29:C33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24:C28 C3:C21 C33:C37">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>